<commit_message>
Update IFDC_fonction de recherche.xlsx
</commit_message>
<xml_diff>
--- a/IFDC_fonction de recherche.xlsx
+++ b/IFDC_fonction de recherche.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView minimized="1" xWindow="120" yWindow="30" windowWidth="15240" windowHeight="3630" firstSheet="6" activeTab="6"/>
+    <workbookView xWindow="120" yWindow="30" windowWidth="15240" windowHeight="3630" firstSheet="5" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="RECHERCHEV 1" sheetId="9" r:id="rId1"/>
@@ -19,7 +19,6 @@
     <sheet name="INDEX" sheetId="16" r:id="rId5"/>
     <sheet name="INDEX-EQUIV" sheetId="15" r:id="rId6"/>
     <sheet name="Excercice" sheetId="18" r:id="rId7"/>
-    <sheet name="Feuil1" sheetId="19" r:id="rId8"/>
   </sheets>
   <definedNames>
     <definedName name="alphabet">#REF!</definedName>
@@ -43,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="216" uniqueCount="112">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="207" uniqueCount="107">
   <si>
     <t>Note</t>
   </si>
@@ -348,12 +347,6 @@
     <t>résultat</t>
   </si>
   <si>
-    <t xml:space="preserve">Interface de consultation </t>
-  </si>
-  <si>
-    <t>Résultat</t>
-  </si>
-  <si>
     <t>CIMENT</t>
   </si>
   <si>
@@ -361,15 +354,6 @@
   </si>
   <si>
     <t>OIGNON</t>
-  </si>
-  <si>
-    <t>selectionnez un produit</t>
-  </si>
-  <si>
-    <t>Selectionnez un trimestre</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Selectionnez une région </t>
   </si>
   <si>
     <t>°</t>
@@ -385,7 +369,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -428,13 +412,6 @@
       <b/>
       <sz val="11"/>
       <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -514,7 +491,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -529,7 +506,6 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -1203,7 +1179,7 @@
         <v>12</v>
       </c>
       <c r="E1" t="s">
-        <v>110</v>
+        <v>105</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
@@ -1308,7 +1284,7 @@
         <v>41</v>
       </c>
       <c r="I7" t="s">
-        <v>109</v>
+        <v>104</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
@@ -1349,18 +1325,18 @@
       <c r="C11" s="2"/>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="D12" s="15" t="s">
+      <c r="D12" s="14" t="s">
         <v>27</v>
       </c>
-      <c r="E12" s="16" t="s">
+      <c r="E12" s="15" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="D14" s="13" t="s">
+      <c r="D14" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="E14" s="14">
+      <c r="E14" s="13">
         <f>IFERROR(VLOOKUP(E12,base_donnee,2,FALSE),"valeur introuvable")</f>
         <v>8</v>
       </c>
@@ -1370,28 +1346,28 @@
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="D15" s="13" t="s">
+      <c r="D15" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="E15" s="14">
+      <c r="E15" s="13">
         <f>IFERROR(VLOOKUP(E12,base_donnee,3,FALSE),"valeur introuvable")</f>
         <v>3715</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="D16" s="13" t="s">
+      <c r="D16" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="E16" s="14">
+      <c r="E16" s="13">
         <f>IFERROR(VLOOKUP(E12,base_donnee,4,FALSE),"valeur introuvable")</f>
         <v>439453</v>
       </c>
     </row>
     <row r="17" spans="4:5" x14ac:dyDescent="0.25">
-      <c r="D17" s="13" t="s">
-        <v>111</v>
-      </c>
-      <c r="E17" s="14" t="str">
+      <c r="D17" s="12" t="s">
+        <v>106</v>
+      </c>
+      <c r="E17" s="13" t="str">
         <f>IFERROR(VLOOKUP(E12,base_donnee,5,FALSE),"valeur introuvable")</f>
         <v>Antananarivo</v>
       </c>
@@ -1727,8 +1703,8 @@
       <c r="J2" s="4" t="s">
         <v>91</v>
       </c>
-      <c r="K2" s="17"/>
-      <c r="L2" s="17"/>
+      <c r="K2" s="16"/>
+      <c r="L2" s="16"/>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3">
@@ -2422,20 +2398,20 @@
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="9" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A9" s="18" t="s">
-        <v>103</v>
-      </c>
-      <c r="B9" s="18"/>
-      <c r="C9" s="18"/>
-      <c r="D9" s="18"/>
-      <c r="E9" s="18"/>
-      <c r="H9" s="18" t="s">
-        <v>104</v>
-      </c>
-      <c r="I9" s="18"/>
-      <c r="J9" s="18"/>
-      <c r="K9" s="18"/>
-      <c r="L9" s="18"/>
+      <c r="A9" s="17" t="s">
+        <v>101</v>
+      </c>
+      <c r="B9" s="17"/>
+      <c r="C9" s="17"/>
+      <c r="D9" s="17"/>
+      <c r="E9" s="17"/>
+      <c r="H9" s="17" t="s">
+        <v>102</v>
+      </c>
+      <c r="I9" s="17"/>
+      <c r="J9" s="17"/>
+      <c r="K9" s="17"/>
+      <c r="L9" s="17"/>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10" s="3"/>
@@ -2850,20 +2826,20 @@
       </c>
     </row>
     <row r="25" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A25" s="18" t="s">
+      <c r="A25" s="17" t="s">
         <v>85</v>
       </c>
-      <c r="B25" s="18"/>
-      <c r="C25" s="18"/>
-      <c r="D25" s="18"/>
-      <c r="E25" s="18"/>
-      <c r="H25" s="18" t="s">
-        <v>105</v>
-      </c>
-      <c r="I25" s="18"/>
-      <c r="J25" s="18"/>
-      <c r="K25" s="18"/>
-      <c r="L25" s="18"/>
+      <c r="B25" s="17"/>
+      <c r="C25" s="17"/>
+      <c r="D25" s="17"/>
+      <c r="E25" s="17"/>
+      <c r="H25" s="17" t="s">
+        <v>103</v>
+      </c>
+      <c r="I25" s="17"/>
+      <c r="J25" s="17"/>
+      <c r="K25" s="17"/>
+      <c r="L25" s="17"/>
     </row>
     <row r="26" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A26" s="3"/>
@@ -3287,106 +3263,4 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I7"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="33" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>106</v>
-      </c>
-      <c r="B3" s="12"/>
-      <c r="C3" s="12"/>
-      <c r="D3" s="12"/>
-      <c r="E3" s="12"/>
-      <c r="F3" s="12" t="s">
-        <v>103</v>
-      </c>
-      <c r="G3" s="12">
-        <v>1</v>
-      </c>
-      <c r="H3" s="12"/>
-      <c r="I3" s="12"/>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>107</v>
-      </c>
-      <c r="B4" s="12"/>
-      <c r="C4" s="12"/>
-      <c r="D4" s="12"/>
-      <c r="E4" s="12"/>
-      <c r="F4" s="12" t="s">
-        <v>104</v>
-      </c>
-      <c r="G4" s="12">
-        <v>2</v>
-      </c>
-      <c r="H4" s="12"/>
-      <c r="I4" s="12"/>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>108</v>
-      </c>
-      <c r="B5" s="12"/>
-      <c r="C5" s="12"/>
-      <c r="D5" s="12"/>
-      <c r="E5" s="12"/>
-      <c r="F5" s="12" t="s">
-        <v>85</v>
-      </c>
-      <c r="G5" s="12">
-        <v>3</v>
-      </c>
-      <c r="H5" s="12"/>
-      <c r="I5" s="12"/>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B6" s="12"/>
-      <c r="C6" s="12"/>
-      <c r="D6" s="12"/>
-      <c r="E6" s="12"/>
-      <c r="F6" s="12" t="s">
-        <v>105</v>
-      </c>
-      <c r="G6" s="12">
-        <v>4</v>
-      </c>
-      <c r="H6" s="12"/>
-      <c r="I6" s="12"/>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A7" s="6" t="s">
-        <v>102</v>
-      </c>
-      <c r="B7" s="12"/>
-      <c r="C7" s="12"/>
-      <c r="D7" s="12"/>
-      <c r="E7" s="12"/>
-      <c r="F7" s="12"/>
-      <c r="G7" s="12"/>
-      <c r="H7" s="12"/>
-      <c r="I7" s="12"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="0" r:id="rId1"/>
-</worksheet>
 </file>
</xml_diff>